<commit_message>
資料庫user user_credential資料(user id 即lable)
</commit_message>
<xml_diff>
--- a/signature_lable_to_text.xlsx
+++ b/signature_lable_to_text.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\畢專\畢專\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\專題\畢業專題\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BC8C072B-D017-4AF3-8934-030DF9E88C58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B80DBE83-0878-47B1-A9F1-E93F7E93082A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="2340" windowWidth="23256" windowHeight="13176" xr2:uid="{381D915B-ACB0-4C0B-9C59-211CEF4C3DFD}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{381D915B-ACB0-4C0B-9C59-211CEF4C3DFD}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -25,57 +25,157 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
-  <si>
-    <t>id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+  <si>
+    <t>徐乙庭</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>陳育鐸</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>孫詠淳</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>林庠毅</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>account</t>
+  </si>
+  <si>
+    <t>user_salt</t>
+  </si>
+  <si>
+    <t>is_filed</t>
+  </si>
+  <si>
+    <t>id/hash_user_id</t>
+  </si>
+  <si>
+    <t>hash_user_pwd</t>
+  </si>
+  <si>
+    <t>created_at</t>
+  </si>
+  <si>
+    <t>pwd</t>
   </si>
   <si>
     <t>name</t>
+  </si>
+  <si>
+    <t>user1</t>
+  </si>
+  <si>
+    <t>user3</t>
+  </si>
+  <si>
+    <t>jJr2I18X</t>
+  </si>
+  <si>
+    <t>user4</t>
+  </si>
+  <si>
+    <t>mbdUs1ij</t>
+  </si>
+  <si>
+    <t>user5</t>
+  </si>
+  <si>
+    <t>user6</t>
+  </si>
+  <si>
+    <t>DdgeMD9i</t>
+  </si>
+  <si>
+    <t>鄭宇翔</t>
+  </si>
+  <si>
+    <t>fF2KmaN6</t>
+  </si>
+  <si>
+    <t>user8</t>
+  </si>
+  <si>
+    <t>ESEI4lmY</t>
+  </si>
+  <si>
+    <t>user9</t>
+  </si>
+  <si>
+    <t>BlB84olh</t>
+  </si>
+  <si>
+    <t>user2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>徐韻蕎</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>徐乙庭</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>陳育鐸</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>詩驛莛</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>莫凱傑</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>孫詠淳</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>鄭宇翔</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>林'庠毅</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>曾嬿儒</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>gF2kV8yH</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>user7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wISwhs2h</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MYeDRN2U</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>f1f6a33b469846f6b6d91df1822d65a5eb6d5f93f6aecad2c76b07dd374cee0f</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>38f0b2fdd8aee7531ab418b118423f368ab760429123b99886cc2147aadbb467</t>
+  </si>
+  <si>
+    <t>d51027a690a8bc0420a8875afb7bbcf4954cdd7700b3b60fac2c1dc5d52731d9</t>
+  </si>
+  <si>
+    <t>1f3d3a67fa887e1e39ca95f65cb932400f61407fcc78eebec57280bbc77f195e</t>
+  </si>
+  <si>
+    <t>628acd7a67ad1a3600ac8dcd133cab39b8a616fe6d467825d65b7addf024ffca</t>
+  </si>
+  <si>
+    <t>d7e6d3ae7f39f5089aaf61c7d0ff05e6c625815da88b36e5ba903f6d916fed45</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6dbec15151b49781d28083703c6291b83d1dc50497be379fcaf44184c084b554</t>
+  </si>
+  <si>
+    <t>1c7eb08c4282b95d3ca4feb9570905dfd5368242586c58739dbbeacd0affb86c</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9ad7e01c0554ed2c512ba57c3b35f9595b8baae198f7794f8be199a286b2b974</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -88,6 +188,23 @@
       <sz val="9"/>
       <name val="新細明體"/>
       <family val="2"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="新細明體"/>
+      <family val="1"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="新細明體"/>
+      <family val="1"/>
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
@@ -114,8 +231,17 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -136,9 +262,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 主題">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -176,7 +302,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -282,7 +408,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -424,7 +550,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -432,96 +558,263 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{667CA806-0A25-4550-9540-6836E3C8C993}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:8" ht="33" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="82.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="82.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="B3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2">
+        <v>2222</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="82.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3">
+      <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2">
+        <v>3333</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="82.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4">
+      <c r="B5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2">
+        <v>4444</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="82.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2">
+        <v>5555</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="82.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5">
+      <c r="C7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2">
+        <v>6666</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="82.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>6</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2">
+        <v>7777</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="82.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="C9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2">
+        <v>8888</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="82.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>10</v>
+      <c r="B10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2">
+        <v>9999</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>